<commit_message>
Updated broken characters in info and online tab
</commit_message>
<xml_diff>
--- a/info.xlsx
+++ b/info.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/royfr474/github/workshop-ngsintro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B438E664-41DF-954B-AECB-644BCD205DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A077FE-2DA1-2E4C-AA84-2B548D0EAD42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5720" yWindow="4760" windowWidth="28040" windowHeight="17440" xr2:uid="{5F8B95CE-8379-E541-8BD7-284A0F505EB1}"/>
+    <workbookView xWindow="14640" yWindow="7140" windowWidth="45440" windowHeight="17440" xr2:uid="{5F8B95CE-8379-E541-8BD7-284A0F505EB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="info" localSheetId="0">Sheet1!$A$1:$H$24</definedName>
+    <definedName name="info" localSheetId="0">Sheet1!$A$1:$H$13</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,7 +40,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{ED5DF6B8-1C55-A94C-8641-5E11DDB739A3}" name="info" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/royfr474/github/workshop-ngsintro/info.csv" tab="0" semicolon="1">
+    <textPr sourceFile="/Users/royfr474/github/workshop-ngsintro/info.csv" tab="0" semicolon="1">
       <textFields count="8">
         <textField/>
         <textField/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="43">
   <si>
     <t>location</t>
   </si>
@@ -92,96 +92,36 @@
     <t>red</t>
   </si>
   <si>
-    <t>Room Retina D227, Building D, Department of Biology, S√∂lvegatan 35, 223 62 Lund, Sweden</t>
-  </si>
-  <si>
     <t>Venue</t>
   </si>
   <si>
-    <t>For Lund city buses, tram, regional buses and regional trains, [click here](https://www.skanetrafiken.se/). You can buy a ticket at the central station in Lund or at the regional bus (card only). You can also use the app [Sk√•netrafiken](https://www.skanetrafiken.se/biljetter/app2/) From the Lund C the easiest is to take the tram from **Clemens torget** towards **ESS** and get off at  **Lund LTH**. The trip take about 4 minutes and a tram leaves about four times an hour.</t>
-  </si>
-  <si>
     <t>umea</t>
   </si>
   <si>
-    <t>Room [UB341](https://link.mazemap.com/7B5bpeV4), Universitetsbibioteket plan 3, Ume√• University, 901 87 Ume√•, Sweden</t>
-  </si>
-  <si>
-    <t>[**Ume√• city buses**](http://tabussen.nu/ultra/english/):&lt;br&gt;There are several options to pay your bus ticket, including on the bus (credit card only) or in advance either online or using the app, or in the ticket machines at Vasaplan or Ume√• Airport. It is cheaper to buy the ticket in advance. More information can be found at [Ultra](https://www.tabussen.nu/ultra/english/where-can-i-buy-tickets/)‚Äôs homepage. The bus stop in the city centre is **Vasaplan** and the stops near the course venue are either **Universum** (buses 2, 5, 8 or 9) or **Samh√§llsvetarhuset** (bus 1). The trip takes about 6-7 min.&lt;br&gt;&lt;br&gt;[**Airport bus**](https://www.tabussen.nu/flygbussen/english/):&lt;br&gt;The airport bus (Bus 80) goes from the airport to **Vasaplan** (the city centre), and takes about 8 min. The [travel planner](https://www.tabussen.nu/ultra/planera-resa/) can be used to plan your trip.</t>
-  </si>
-  <si>
     <t>uppsala</t>
   </si>
   <si>
     <t>Room [E10:1309](https://link.mazemap.com/Wza07nfx), Entrance C11, Biomedicinskt centrum, Uppsala University / ScilifeLab, Husargatan 3, 75237 Uppsala, Sweden</t>
   </si>
   <si>
-    <t>Few selected hotels are listed below ranked by distance from the venue.</t>
-  </si>
-  <si>
-    <t>- [Hotel von Kraemer](https://hotelvonkraemer.se/) (900 m, 11 min walk)</t>
-  </si>
-  <si>
-    <t>- [Akademihotellet](https://akademihotellet.se/en/) (1.7 Km, 21 min walk)</t>
-  </si>
-  <si>
-    <t>- [CityStay Hotell](https://citystayuppsala.se/) (1.8 Km, 21 min walk)</t>
-  </si>
-  <si>
-    <t>- [Grand Hotel H√∂rnan](https://www.grandhotellhornan.com/) (1.9 Km, 23 min walk)</t>
-  </si>
-  <si>
-    <t>- [Hotell Centralstation](http://hotellcentralstation.se/) (2.1 Km, 25 min walk)</t>
-  </si>
-  <si>
-    <t>- [Best Western Svava](https://www.hotelsvava.se/) (2.2 Km, 26 min walk)</t>
-  </si>
-  <si>
-    <t>The venue and hotels are also marked on the map.</t>
-  </si>
-  <si>
-    <t>Use the [UL website](https://www.ul.se) or the [UL app](https://www.ul.se/en/tickets/how-to-buy-a-ticket/the-UL-app/) for bus and train services around Uppsala. For buses from the Centralstation (Train/Bus), take Bus 4 (towards **Gottsunda Centrum**) or 8 (towards **Sunnersta**) and get off at the stop **Uppsala Science Park**. Bus tickets can be purchased in the app or directly from the driver using a credit card."</t>
-  </si>
-  <si>
     <t>bed</t>
   </si>
   <si>
     <t>blue</t>
   </si>
   <si>
-    <t>von Kraemers all√© 26, 75237 Uppsala, 900 m (11 min walk)</t>
-  </si>
-  <si>
     <t>Hotel von Kraemer</t>
   </si>
   <si>
-    <t>Bang√•rdsgatan 1, 75320 Uppsala, 1.9 Km (23 min walk)</t>
-  </si>
-  <si>
-    <t>Grand Hotell H√∂rnan</t>
-  </si>
-  <si>
-    <t>√ñvre Slottsgatan 5, 75310 Uppsala, 1.7 Km (21 min walk)</t>
-  </si>
-  <si>
     <t>Akademihotellet</t>
   </si>
   <si>
-    <t>Bang√•rdsgatan 24, 75320 Uppsala, 2.2 Km (26 min walk)</t>
-  </si>
-  <si>
     <t>Best Western Hotel Svava</t>
   </si>
   <si>
-    <t>Bang√•rdsgatan 13, 753 30 Uppsala, 2.1 Km (25 min walk)</t>
-  </si>
-  <si>
     <t>Hotell Centralstation</t>
   </si>
   <si>
-    <t>Tr√§dg√•rdsgatan 5A, 753 09 Uppsala, 1.8 Km (21 min walk)</t>
-  </si>
-  <si>
     <t>CityStay Hotell</t>
   </si>
   <si>
@@ -200,16 +140,60 @@
     <t>linkoping</t>
   </si>
   <si>
-    <t>Campus Valla, C-house, Entrance 12, 581 83 Link√∂ping, Sweden</t>
-  </si>
-  <si>
-    <t>Use the [√ñstg√∂tatrafiken website](https://www.ostgotatrafiken.se) or the [√ñstg√∂tatrafiken app](https://www.ostgotatrafiken.se/kundservice/hur-kan-vi-hjalpa-dig/nya-appen/) for bus services around Link√∂ping. The easiest way to by tickets is through the app, but you can by a travel card in advance which you can load with tickets as described [here](https://www.ostgotatrafiken.se/biljetter/kopa-biljett/utan-app/). From Link√∂ping Resecentrum, take bus 12 (towards Lambohov) or bus 543 (towards Slaka) and get off at the stop *M√§ster Mattias v√§g*.</t>
-  </si>
-  <si>
     <t>online</t>
   </si>
   <si>
-    <t>The workshop is online only. Online meeting links are sent to participants by email.</t>
+    <t>von Kraemers alle 26, 75237 Uppsala, 900 m (11 min walk)</t>
+  </si>
+  <si>
+    <t>Grand Hotell Hörnan</t>
+  </si>
+  <si>
+    <t>Bangårdsgatan 1, 753 20 Uppsala, 1.9 Km (23 min walk)</t>
+  </si>
+  <si>
+    <t>Övre Slottsgatan 5, 753 10 Uppsala, 1.7 Km (21 min walk)</t>
+  </si>
+  <si>
+    <t>Bangårdsgatan 24, 753 20 Uppsala, 2.2 Km (26 min walk)</t>
+  </si>
+  <si>
+    <t>Bangårdsgatan 13, 753 30 Uppsala, 2.1 Km (25 min walk)</t>
+  </si>
+  <si>
+    <t>Trädgårdsgatan 5A, 753 09 Uppsala, 1.8 Km (21 min walk)</t>
+  </si>
+  <si>
+    <t>Campus Valla, C-house, Entrance 12, 581 83 Linköping, Sweden</t>
+  </si>
+  <si>
+    <t>Room Retina D227, Building D, Department of Biology, Sölvegatan 35, 223 62 Lund, Sweden</t>
+  </si>
+  <si>
+    <t>Room [UB341](https://link.mazemap.com/7B5bpeV4), Universitetsbibioteket plan 3, Umeå University, 901 87 Umeå, Sweden</t>
+  </si>
+  <si>
+    <t>Few selected hotels are listed below ranked by distance from the venue.
+- [Hotel von Kraemer](https://hotelvonkraemer.se/) (900 m, 11 min walk)
+- [Akademihotellet](https://akademihotellet.se/en/) (1.7 Km, 21 min walk)
+- [CityStay Hotell](https://citystayuppsala.se/) (1.8 Km, 21 min walk)
+- [Grand Hotel Hörnan](https://www.grandhotellhornan.com/) (1.9 Km, 23 min walk)
+- [Hotell Centralstation](http://hotellcentralstation.se/) (2.1 Km, 25 min walk)
+- [Best Western Svava](https://www.hotelsvava.se/) (2.2 Km, 26 min walk)
+The venue and hotels are also marked on the map.
+Use the [UL website](https://www.ul.se) or the [UL app](https://www.ul.se/en/tickets/how-to-buy-a-ticket/the-UL-app/) for bus and train services around Uppsala. For buses from the Centralstation (Train/Bus), take Bus 4 (towards **Gottsunda Centrum**) or 8 (towards **Sunnersta**) and get off at the stop **Uppsala Science Park**. Bus tickets can be purchased in the app or directly from the driver using a credit card.</t>
+  </si>
+  <si>
+    <t>Use the [östgötatrafiken website](https://www.ostgotatrafiken.se) or the [östgötatrafiken app](https://www.ostgotatrafiken.se/kundservice/hur-kan-vi-hjalpa-dig/nya-appen/) for bus services around Linköping. The easiest way to by tickets is through the app, but you can by a travel card in advance which you can load with tickets as described [here](https://www.ostgotatrafiken.se/biljetter/kopa-biljett/utan-app/). From Linköping Resecentrum, take bus 12 (towards Lambohov) or bus 543 (towards Slaka) and get off at the stop **Mäster Mattias väg**.</t>
+  </si>
+  <si>
+    <t>For Lund city buses, tram, regional buses and regional trains, use [skanetrafiken.se](https://www.skanetrafiken.se/). You can buy a ticket at the central station in Lund or at the regional bus (card only). You can also use the app [Skånetrafiken](https://www.skanetrafiken.se/biljetter/app2/) From the Lund C the easiest is to take the tram from **Clemens torget** towards **ESS** and get off at  **Lund LTH**. The trip take about 4 minutes and a tram leaves about four times an hour.</t>
+  </si>
+  <si>
+    <t>[**Umeå city buses**](http://tabussen.nu/ultra/english/):&lt;br&gt;There are several options to pay your bus ticket, including on the bus (credit card only) or in advance either online or using the app, or in the ticket machines at Vasaplan or Umeå Airport. It is cheaper to buy the ticket in advance. More information can be found at [Ultra](https://www.tabussen.nu/ultra/english/where-can-i-buy-tickets/)'s homepage. The bus stop in the city centre is **Vasaplan** and the stops near the course venue are either **Universum** (buses 2, 5, 8 or 9) or **Samhällsvetarhuset** (bus 1). The trip takes about 6-7 min.&lt;br&gt;&lt;br&gt;[**Airport bus**](https://www.tabussen.nu/flygbussen/english/):&lt;br&gt;The airport bus (Bus 80) goes from the airport to **Vasaplan** (the city centre), and takes about 8 min. The [travel planner](https://www.tabussen.nu/ultra/planera-resa/) can be used to plan your trip.</t>
+  </si>
+  <si>
+    <t>Online meeting links are sent to participants by email.</t>
   </si>
 </sst>
 </file>
@@ -245,8 +229,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -565,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C682103A-4E94-8940-91C1-6B6AF5A5418B}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -625,18 +612,18 @@
         <v>13.206628</v>
       </c>
       <c r="F2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -651,18 +638,18 @@
         <v>20.307814</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="272" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -677,248 +664,208 @@
         <v>17.637073000000001</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" t="s">
-        <v>19</v>
+        <v>11</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5">
+        <v>59.8486686913499</v>
+      </c>
+      <c r="E5">
+        <v>17.6352515582604</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>59.856544126786901</v>
+      </c>
+      <c r="E6">
+        <v>17.640590387880302</v>
+      </c>
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7">
+        <v>59.856594256720101</v>
+      </c>
+      <c r="E7">
+        <v>17.630563108921201</v>
+      </c>
+      <c r="F7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8">
+        <v>59.858191861161899</v>
+      </c>
+      <c r="E8">
+        <v>17.644074126326402</v>
+      </c>
+      <c r="F8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9">
+        <v>59.858300986485197</v>
+      </c>
+      <c r="E9">
+        <v>17.644077842083998</v>
+      </c>
+      <c r="F9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10">
+        <v>59.857091713462502</v>
+      </c>
+      <c r="E10">
+        <v>17.635753423926001</v>
+      </c>
+      <c r="F10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11">
+        <v>59.858555236329899</v>
+      </c>
+      <c r="E11">
+        <v>17.645584924846901</v>
+      </c>
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>58.402748000000003</v>
+      </c>
+      <c r="E12">
+        <v>15.578822000000001</v>
+      </c>
+      <c r="F12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16">
-        <v>59.8486686913499</v>
-      </c>
-      <c r="E16">
-        <v>17.6352515582604</v>
-      </c>
-      <c r="F16" t="s">
-        <v>30</v>
-      </c>
-      <c r="G16" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17">
-        <v>59.856544126786901</v>
-      </c>
-      <c r="E17">
-        <v>17.640590387880302</v>
-      </c>
-      <c r="F17" t="s">
-        <v>32</v>
-      </c>
-      <c r="G17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18">
-        <v>59.856594256720101</v>
-      </c>
-      <c r="E18">
-        <v>17.630563108921201</v>
-      </c>
-      <c r="F18" t="s">
-        <v>34</v>
-      </c>
-      <c r="G18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19">
-        <v>59.858191861161899</v>
-      </c>
-      <c r="E19">
-        <v>17.644074126326402</v>
-      </c>
-      <c r="F19" t="s">
-        <v>36</v>
-      </c>
-      <c r="G19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20">
-        <v>59.858300986485197</v>
-      </c>
-      <c r="E20">
-        <v>17.644077842083998</v>
-      </c>
-      <c r="F20" t="s">
-        <v>38</v>
-      </c>
-      <c r="G20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21">
-        <v>59.857091713462502</v>
-      </c>
-      <c r="E21">
-        <v>17.635753423926001</v>
-      </c>
-      <c r="F21" t="s">
-        <v>40</v>
-      </c>
-      <c r="G21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="H13" t="s">
         <v>42</v>
-      </c>
-      <c r="C22" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22">
-        <v>59.858555236329899</v>
-      </c>
-      <c r="E22">
-        <v>17.645584924846901</v>
-      </c>
-      <c r="F22" t="s">
-        <v>44</v>
-      </c>
-      <c r="G22" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23">
-        <v>58.402748000000003</v>
-      </c>
-      <c r="E23">
-        <v>15.578822000000001</v>
-      </c>
-      <c r="F23" t="s">
-        <v>47</v>
-      </c>
-      <c r="G23" t="s">
-        <v>12</v>
-      </c>
-      <c r="H23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>49</v>
-      </c>
-      <c r="H24" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated uppmax project and venue address
</commit_message>
<xml_diff>
--- a/info.xlsx
+++ b/info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/royfr474/github/workshop-ngsintro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A077FE-2DA1-2E4C-AA84-2B548D0EAD42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B399EA-FA4F-3A4B-986E-88EFF7B6D41C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14640" yWindow="7140" windowWidth="45440" windowHeight="17440" xr2:uid="{5F8B95CE-8379-E541-8BD7-284A0F505EB1}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" xr2:uid="{5F8B95CE-8379-E541-8BD7-284A0F505EB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -164,9 +164,6 @@
     <t>Trädgårdsgatan 5A, 753 09 Uppsala, 1.8 Km (21 min walk)</t>
   </si>
   <si>
-    <t>Campus Valla, C-house, Entrance 12, 581 83 Linköping, Sweden</t>
-  </si>
-  <si>
     <t>Room Retina D227, Building D, Department of Biology, Sölvegatan 35, 223 62 Lund, Sweden</t>
   </si>
   <si>
@@ -194,6 +191,14 @@
   </si>
   <si>
     <t>Online meeting links are sent to participants by email.</t>
+  </si>
+  <si>
+    <t>LiU Campus Universitetssjukhuset
+58225 Linköping
+Sweden
+Monday-Tuesday: [Room Papaver, Hus 511/001](https://link.mazemap.com/00mnumNU)
+Wednesday-Thursday: [Room Dolomit, Hus 440](https://link.mazemap.com/up3GnjPm)
+Friday: [Room Antracit, Hus 440](https://link.mazemap.com/wXeFDYNR)</t>
   </si>
 </sst>
 </file>
@@ -555,7 +560,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -612,13 +617,13 @@
         <v>13.206628</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -638,13 +643,13 @@
         <v>20.307814</v>
       </c>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="272" x14ac:dyDescent="0.2">
@@ -670,7 +675,7 @@
         <v>11</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -834,7 +839,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="119" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -845,19 +850,19 @@
         <v>10</v>
       </c>
       <c r="D12">
-        <v>58.402748000000003</v>
+        <v>58.403739645581503</v>
       </c>
       <c r="E12">
-        <v>15.578822000000001</v>
-      </c>
-      <c r="F12" t="s">
-        <v>35</v>
+        <v>15.6223647575603</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="G12" t="s">
         <v>11</v>
       </c>
       <c r="H12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -865,10 +870,11 @@
         <v>27</v>
       </c>
       <c r="H13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added popup for info, Delimiter changed to semicolon, Updated schedule, info
</commit_message>
<xml_diff>
--- a/info.xlsx
+++ b/info.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/royfr474/github/workshop-ngsintro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B399EA-FA4F-3A4B-986E-88EFF7B6D41C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{812FCB34-28B7-6845-A656-87F285C7B3DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" xr2:uid="{5F8B95CE-8379-E541-8BD7-284A0F505EB1}"/>
+    <workbookView xWindow="4340" yWindow="5480" windowWidth="36000" windowHeight="22500" xr2:uid="{5F8B95CE-8379-E541-8BD7-284A0F505EB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="info" localSheetId="0">Sheet1!$A$1:$H$13</definedName>
+    <definedName name="info" localSheetId="0">Sheet1!$A$1:$I$13</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,6 +35,49 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Roy Francis</author>
+  </authors>
+  <commentList>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{FFCA34FA-7A34-BA43-86FE-CDE1A4BB6A28}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Roy Francis:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Semicolon inserts linebreaks in HTML</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
@@ -57,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
   <si>
     <t>location</t>
   </si>
@@ -101,9 +144,6 @@
     <t>uppsala</t>
   </si>
   <si>
-    <t>Room [E10:1309](https://link.mazemap.com/Wza07nfx), Entrance C11, Biomedicinskt centrum, Uppsala University / ScilifeLab, Husargatan 3, 75237 Uppsala, Sweden</t>
-  </si>
-  <si>
     <t>bed</t>
   </si>
   <si>
@@ -131,9 +171,6 @@
     <t>green</t>
   </si>
   <si>
-    <t>Central Station, 753 21 Uppsala</t>
-  </si>
-  <si>
     <t>Central station</t>
   </si>
   <si>
@@ -143,31 +180,7 @@
     <t>online</t>
   </si>
   <si>
-    <t>von Kraemers alle 26, 75237 Uppsala, 900 m (11 min walk)</t>
-  </si>
-  <si>
     <t>Grand Hotell Hörnan</t>
-  </si>
-  <si>
-    <t>Bangårdsgatan 1, 753 20 Uppsala, 1.9 Km (23 min walk)</t>
-  </si>
-  <si>
-    <t>Övre Slottsgatan 5, 753 10 Uppsala, 1.7 Km (21 min walk)</t>
-  </si>
-  <si>
-    <t>Bangårdsgatan 24, 753 20 Uppsala, 2.2 Km (26 min walk)</t>
-  </si>
-  <si>
-    <t>Bangårdsgatan 13, 753 30 Uppsala, 2.1 Km (25 min walk)</t>
-  </si>
-  <si>
-    <t>Trädgårdsgatan 5A, 753 09 Uppsala, 1.8 Km (21 min walk)</t>
-  </si>
-  <si>
-    <t>Room Retina D227, Building D, Department of Biology, Sölvegatan 35, 223 62 Lund, Sweden</t>
-  </si>
-  <si>
-    <t>Room [UB341](https://link.mazemap.com/7B5bpeV4), Universitetsbibioteket plan 3, Umeå University, 901 87 Umeå, Sweden</t>
   </si>
   <si>
     <t>Few selected hotels are listed below ranked by distance from the venue.
@@ -181,9 +194,6 @@
 Use the [UL website](https://www.ul.se) or the [UL app](https://www.ul.se/en/tickets/how-to-buy-a-ticket/the-UL-app/) for bus and train services around Uppsala. For buses from the Centralstation (Train/Bus), take Bus 4 (towards **Gottsunda Centrum**) or 8 (towards **Sunnersta**) and get off at the stop **Uppsala Science Park**. Bus tickets can be purchased in the app or directly from the driver using a credit card.</t>
   </si>
   <si>
-    <t>Use the [östgötatrafiken website](https://www.ostgotatrafiken.se) or the [östgötatrafiken app](https://www.ostgotatrafiken.se/kundservice/hur-kan-vi-hjalpa-dig/nya-appen/) for bus services around Linköping. The easiest way to by tickets is through the app, but you can by a travel card in advance which you can load with tickets as described [here](https://www.ostgotatrafiken.se/biljetter/kopa-biljett/utan-app/). From Linköping Resecentrum, take bus 12 (towards Lambohov) or bus 543 (towards Slaka) and get off at the stop **Mäster Mattias väg**.</t>
-  </si>
-  <si>
     <t>For Lund city buses, tram, regional buses and regional trains, use [skanetrafiken.se](https://www.skanetrafiken.se/). You can buy a ticket at the central station in Lund or at the regional bus (card only). You can also use the app [Skånetrafiken](https://www.skanetrafiken.se/biljetter/app2/) From the Lund C the easiest is to take the tram from **Clemens torget** towards **ESS** and get off at  **Lund LTH**. The trip take about 4 minutes and a tram leaves about four times an hour.</t>
   </si>
   <si>
@@ -193,25 +203,86 @@
     <t>Online meeting links are sent to participants by email.</t>
   </si>
   <si>
-    <t>LiU Campus Universitetssjukhuset
-58225 Linköping
-Sweden
-Monday-Tuesday: [Room Papaver, Hus 511/001](https://link.mazemap.com/00mnumNU)
-Wednesday-Thursday: [Room Dolomit, Hus 440](https://link.mazemap.com/up3GnjPm)
+    <t>popup</t>
+  </si>
+  <si>
+    <t>Room Retina D227; Building D; Department of Biology; Sölvegatan 35; 223 62 Lund, Sweden</t>
+  </si>
+  <si>
+    <t>Room [UB341](https://link.mazemap.com/7B5bpeV4); Universitetsbibioteket plan 3; Umeå University; 901 87 Umeå; Sweden</t>
+  </si>
+  <si>
+    <t>Room UB341; Universitetsbibioteket plan 3; Umeå University; 901 87 Umeå; Sweden</t>
+  </si>
+  <si>
+    <t>Room [E10:1309](https://link.mazemap.com/Wza07nfx); Entrance C11; Biomedicinskt centrum; Uppsala University / ScilifeLab; Husargatan 3; 75237 Uppsala; Sweden</t>
+  </si>
+  <si>
+    <t>Room E10:1309; Entrance C11; Biomedicinskt centrum; Uppsala University / ScilifeLab; Husargatan 3; 75237 Uppsala; Sweden</t>
+  </si>
+  <si>
+    <t>von Kraemers alle 26; 75237 Uppsala; 900 m (11 min walk)</t>
+  </si>
+  <si>
+    <t>Bangårdsgatan 1; 753 20 Uppsala; 1.9 Km (23 min walk)</t>
+  </si>
+  <si>
+    <t>Övre Slottsgatan 5; 753 10 Uppsala; 1.7 Km (21 min walk)</t>
+  </si>
+  <si>
+    <t>Bangårdsgatan 24; 753 20 Uppsala; 2.2 Km (26 min walk)</t>
+  </si>
+  <si>
+    <t>Bangårdsgatan 13; 753 30 Uppsala; 2.1 Km (25 min walk)</t>
+  </si>
+  <si>
+    <t>Trädgårdsgatan 5A; 753 09 Uppsala; 1.8 Km (21 min walk)</t>
+  </si>
+  <si>
+    <t>Central Station; 753 21 Uppsala</t>
+  </si>
+  <si>
+    <t>LiU Campus Universitetssjukhuset; 58225 Linköping; Sweden;
+;
+Monday-Tuesday: [Room Papaver, Hus 511/001](https://link.mazemap.com/00mnumNU);
+Wednesday-Thursday: [Room Dolomit, Hus 440](https://link.mazemap.com/up3GnjPm);
 Friday: [Room Antracit, Hus 440](https://link.mazemap.com/wXeFDYNR)</t>
+  </si>
+  <si>
+    <t>LiU Campus Universitetssjukhuset; 58225 Linköping; Sweden;
+;
+Monday-Tuesday: Room Papaver, Hus 511/001;
+Wednesday-Thursday: Room Dolomit, Hus 440;
+Friday: Room Antracit, Hus 440</t>
+  </si>
+  <si>
+    <t>Use the [östgötatrafiken website](https://www.ostgotatrafiken.se) or the [östgötatrafiken app](https://www.ostgotatrafiken.se/kundservice/hur-kan-vi-hjalpa-dig/nya-appen/) for bus services around Linköping. The easiest way to by tickets is through the app, but you can by a travel card in advance which you can load with tickets.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -556,11 +627,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C682103A-4E94-8940-91C1-6B6AF5A5418B}">
-  <dimension ref="A1:H13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C682103A-4E94-8940-91C1-6B6AF5A5418B}">
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -570,11 +641,12 @@
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="80.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="59.5" customWidth="1"/>
+    <col min="8" max="8" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="80.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -594,13 +666,16 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -617,16 +692,19 @@
         <v>13.206628</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -643,16 +721,19 @@
         <v>20.307814</v>
       </c>
       <c r="F3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" t="s">
         <v>11</v>
       </c>
-      <c r="H3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="272" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="272" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -669,24 +750,27 @@
         <v>17.637073000000001</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="G4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
         <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
       </c>
       <c r="D5">
         <v>59.8486686913499</v>
@@ -695,21 +779,24 @@
         <v>17.6352515582604</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="G5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="H5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
         <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
       </c>
       <c r="D6">
         <v>59.856544126786901</v>
@@ -718,21 +805,24 @@
         <v>17.640590387880302</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="H6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
         <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
       </c>
       <c r="D7">
         <v>59.856594256720101</v>
@@ -741,21 +831,24 @@
         <v>17.630563108921201</v>
       </c>
       <c r="F7" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="H7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
       <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
         <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
       </c>
       <c r="D8">
         <v>59.858191861161899</v>
@@ -764,21 +857,24 @@
         <v>17.644074126326402</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="G8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="H8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
       <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
         <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>16</v>
       </c>
       <c r="D9">
         <v>59.858300986485197</v>
@@ -787,21 +883,24 @@
         <v>17.644077842083998</v>
       </c>
       <c r="F9" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="G9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="H9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
       <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
         <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
       </c>
       <c r="D10">
         <v>59.857091713462502</v>
@@ -810,21 +909,24 @@
         <v>17.635753423926001</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="G10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="H10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
         <v>22</v>
-      </c>
-      <c r="C11" t="s">
-        <v>23</v>
       </c>
       <c r="D11">
         <v>59.858555236329899</v>
@@ -833,15 +935,18 @@
         <v>17.645584924846901</v>
       </c>
       <c r="F11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="85" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>24</v>
-      </c>
-      <c r="G11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="119" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>26</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
@@ -850,31 +955,35 @@
         <v>10</v>
       </c>
       <c r="D12">
-        <v>58.403739645581503</v>
+        <v>58.403544601115797</v>
       </c>
       <c r="E12">
-        <v>15.6223647575603</v>
+        <v>15.6221650546244</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" t="s">
         <v>11</v>
       </c>
-      <c r="H12" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H13" t="s">
-        <v>41</v>
+        <v>25</v>
+      </c>
+      <c r="I13" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated map, restaurant and minor fixes
</commit_message>
<xml_diff>
--- a/info.xlsx
+++ b/info.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/royfr474/github/workshop-ngsintro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{812FCB34-28B7-6845-A656-87F285C7B3DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB3D194-9D0D-D543-BD18-B5E5F57D4666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="5480" windowWidth="36000" windowHeight="22500" xr2:uid="{5F8B95CE-8379-E541-8BD7-284A0F505EB1}"/>
+    <workbookView xWindow="37000" yWindow="3160" windowWidth="36000" windowHeight="22500" xr2:uid="{5F8B95CE-8379-E541-8BD7-284A0F505EB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="info" localSheetId="0">Sheet1!$A$1:$I$13</definedName>
+    <definedName name="info" localSheetId="0">Sheet1!$A$1:$I$18</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -43,6 +43,73 @@
     <author>Roy Francis</author>
   </authors>
   <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{C0F541EB-D483-E348-ACA5-261EEF9A2E72}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Roy Francis:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">fontawesome v4
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{048DA6C6-3B9A-6846-A6E4-D5AF9807EA68}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Roy Francis:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>See documentation for awesomeIcons</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="F1" authorId="0" shapeId="0" xr:uid="{FFCA34FA-7A34-BA43-86FE-CDE1A4BB6A28}">
       <text>
         <r>
@@ -100,7 +167,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="58">
   <si>
     <t>location</t>
   </si>
@@ -257,6 +324,49 @@
   </si>
   <si>
     <t>Use the [östgötatrafiken website](https://www.ostgotatrafiken.se) or the [östgötatrafiken app](https://www.ostgotatrafiken.se/kundservice/hur-kan-vi-hjalpa-dig/nya-appen/) for bus services around Linköping. The easiest way to by tickets is through the app, but you can by a travel card in advance which you can load with tickets.</t>
+  </si>
+  <si>
+    <t>Pappa Grappa restaurant; Hospitalsgränd 1; 582 27 Linköping</t>
+  </si>
+  <si>
+    <t>LiU Campus Universitetssjukhuset; 58225 Linköping; Sweden;
+;
+Monday-Tuesday: [Room Papaver, Hus 511/001](https://link.mazemap.com/00mnumNU);</t>
+  </si>
+  <si>
+    <t>LiU Campus Universitetssjukhuset; 58225 Linköping; Sweden;
+;
+Wednesday-Thursday: [Room Dolomit, Hus 440](https://link.mazemap.com/up3GnjPm);
+Friday: [Room Antracit, Hus 440](https://link.mazemap.com/wXeFDYNR)</t>
+  </si>
+  <si>
+    <t>LiU Campus Universitetssjukhuset; 58225 Linköping; Sweden;
+;
+Wednesday-Thursday: Room Dolomit, Hus 440;
+Friday: Room Antracit, Hus 440</t>
+  </si>
+  <si>
+    <t>LiU Campus Universitetssjukhuset; 58225 Linköping; Sweden;
+;
+Monday-Tuesday: Room Papaver, Hus 511/001;</t>
+  </si>
+  <si>
+    <t>Central Station; Järnvägsgatan; 582 22 Linköping</t>
+  </si>
+  <si>
+    <t>purple</t>
+  </si>
+  <si>
+    <t>Quality Hotel Ekoxen; Klostergatan 68; 582 23 Linköping</t>
+  </si>
+  <si>
+    <t>Quality Hotel Ekoxen</t>
+  </si>
+  <si>
+    <t>Pappa Grappa restaurant</t>
+  </si>
+  <si>
+    <t>cutlery</t>
   </si>
 </sst>
 </file>
@@ -628,10 +738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C682103A-4E94-8940-91C1-6B6AF5A5418B}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -926,7 +1036,7 @@
         <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="D11">
         <v>59.858555236329899</v>
@@ -948,18 +1058,6 @@
       <c r="A12" t="s">
         <v>24</v>
       </c>
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12">
-        <v>58.403544601115797</v>
-      </c>
-      <c r="E12">
-        <v>15.6221650546244</v>
-      </c>
       <c r="F12" s="1" t="s">
         <v>44</v>
       </c>
@@ -973,11 +1071,141 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>58.403544601115797</v>
+      </c>
+      <c r="E13">
+        <v>15.6221650546244</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>58.402218182958997</v>
+      </c>
+      <c r="E14">
+        <v>15.6220954584164</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15">
+        <v>58.409715884976499</v>
+      </c>
+      <c r="E15">
+        <v>15.6222992598926</v>
+      </c>
+      <c r="F15" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16">
+        <v>58.405826529222502</v>
+      </c>
+      <c r="E16">
+        <v>15.6252718211986</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17">
+        <v>58.416128036561098</v>
+      </c>
+      <c r="E17">
+        <v>15.626098868559801</v>
+      </c>
+      <c r="F17" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" t="s">
+        <v>52</v>
+      </c>
+      <c r="H17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>25</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I18" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>